<commit_message>
Multiple correct answers for fill the blank
</commit_message>
<xml_diff>
--- a/test_data/A2.1/Лексика/Атмосфера.xlsx
+++ b/test_data/A2.1/Лексика/Атмосфера.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t xml:space="preserve">Текст вопроса</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">sun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sol</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="35.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.24"/>
@@ -221,16 +224,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.02"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,6 +244,9 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -247,6 +254,9 @@
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>